<commit_message>
elsa s01 option class completed.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA.xlsx
+++ b/elsa/doc/Scrum_ELSA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\P06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5237650-F966-43E1-B841-02B1B824F2C5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2C301-FA6A-4FC2-96FA-22A099367725}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="88">
   <si>
     <t>Product Name:</t>
   </si>
@@ -301,9 +301,6 @@
   <si>
     <t>In Work</t>
   </si>
-  <si>
-    <t>In Test</t>
-  </si>
 </sst>
 </file>
 
@@ -559,6 +556,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -570,9 +570,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -783,19 +780,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3032,7 +3029,7 @@
   <dimension ref="A1:AMK96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3055,14 +3052,14 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3" t="s">
         <v>2</v>
@@ -3073,14 +3070,14 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -3119,18 +3116,18 @@
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="40">
         <v>1001520302</v>
       </c>
       <c r="J5" s="2"/>
@@ -3242,11 +3239,11 @@
       </c>
       <c r="B13" s="2">
         <f>B12-C13</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 1")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
@@ -3266,7 +3263,7 @@
       </c>
       <c r="B14" s="2">
         <f>B13-C14</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 2")</f>
@@ -3290,7 +3287,7 @@
       </c>
       <c r="B15" s="2">
         <f>B14-C15</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 3")</f>
@@ -3314,7 +3311,7 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 4")</f>
@@ -3334,7 +3331,7 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 4")</f>
@@ -3406,10 +3403,10 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="43" t="s">
+      <c r="F22" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="43"/>
+      <c r="G22" s="44"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
@@ -3498,7 +3495,7 @@
         <v>2</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>35</v>
@@ -4538,7 +4535,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
elsa s01 desktop class written but not tested.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA.xlsx
+++ b/elsa/doc/Scrum_ELSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E2C301-FA6A-4FC2-96FA-22A099367725}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B45CBF-FC1D-45E5-AE19-814A8F736904}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="88">
   <si>
     <t>Product Name:</t>
   </si>
@@ -299,7 +299,7 @@
     <t>Completed Day 3</t>
   </si>
   <si>
-    <t>In Work</t>
+    <t>In Test</t>
   </si>
 </sst>
 </file>
@@ -1072,19 +1072,19 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3028,8 +3028,8 @@
   </sheetPr>
   <dimension ref="A1:AMK96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3523,7 +3523,9 @@
         <v>8</v>
       </c>
       <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
+      <c r="G26" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="H26" s="19" t="s">
         <v>31</v>
       </c>
@@ -4534,8 +4536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4691,11 +4693,11 @@
       </c>
       <c r="B10" s="33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C10" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="26"/>
@@ -4709,7 +4711,7 @@
       </c>
       <c r="B11" s="33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C11" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -4727,7 +4729,7 @@
       </c>
       <c r="B12" s="33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C12" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -4745,7 +4747,7 @@
       </c>
       <c r="B13" s="33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -4763,7 +4765,7 @@
       </c>
       <c r="B14" s="33">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C14" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -4917,7 +4919,7 @@
         <v>69</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F23" s="38"/>
     </row>
@@ -4932,7 +4934,9 @@
       <c r="D24" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="37"/>
+      <c r="E24" s="37" t="s">
+        <v>86</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6">
@@ -4946,7 +4950,9 @@
       <c r="D25" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="37"/>
+      <c r="E25" s="37" t="s">
+        <v>86</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6">
@@ -4960,7 +4966,9 @@
       <c r="D26" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="37"/>
+      <c r="E26" s="37" t="s">
+        <v>86</v>
+      </c>
       <c r="F26" s="38"/>
     </row>
     <row r="27" spans="1:6">

</xml_diff>

<commit_message>
elsa s01 desktop test passed.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA.xlsx
+++ b/elsa/doc/Scrum_ELSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B45CBF-FC1D-45E5-AE19-814A8F736904}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E6E301-9A45-4E79-A205-1CF5E37E6CA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3048" yWindow="3048" windowWidth="17280" windowHeight="9108" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="88">
   <si>
     <t>Product Name:</t>
   </si>
@@ -299,7 +299,7 @@
     <t>Completed Day 3</t>
   </si>
   <si>
-    <t>In Test</t>
+    <t>In Work</t>
   </si>
 </sst>
 </file>
@@ -780,19 +780,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3028,27 +3028,27 @@
   </sheetPr>
   <dimension ref="A1:AMK96"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="13" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="62.28515625" style="1" customWidth="1"/>
-    <col min="12" max="1025" width="11.5703125" style="1"/>
+    <col min="9" max="9" width="45.5546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="62.33203125" style="1" customWidth="1"/>
+    <col min="12" max="1025" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="18">
+    <row r="1" spans="1:10" s="4" customFormat="1" ht="17.399999999999999">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3066,7 +3066,7 @@
       </c>
       <c r="J1"/>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="15.75">
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="15.6">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3239,11 +3239,11 @@
       </c>
       <c r="B13" s="2">
         <f>B12-C13</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 1")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B14" s="2">
         <f>B13-C14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 2")</f>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="B15" s="2">
         <f>B14-C15</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 3")</f>
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 4")</f>
@@ -3331,7 +3331,7 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 4")</f>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" ht="25.5">
+    <row r="25" spans="1:11" ht="26.4">
       <c r="A25" s="16" t="s">
         <v>34</v>
       </c>
@@ -3508,7 +3508,7 @@
       </c>
       <c r="K25" s="20"/>
     </row>
-    <row r="26" spans="1:11" ht="25.5">
+    <row r="26" spans="1:11" ht="26.4">
       <c r="A26" s="16" t="s">
         <v>38</v>
       </c>
@@ -3524,7 +3524,7 @@
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>31</v>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="K26" s="20"/>
     </row>
-    <row r="27" spans="1:11" ht="25.5">
+    <row r="27" spans="1:11" ht="26.4">
       <c r="A27" s="16" t="s">
         <v>41</v>
       </c>
@@ -3552,7 +3552,9 @@
         <v>13</v>
       </c>
       <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="G27" s="18" t="s">
+        <v>87</v>
+      </c>
       <c r="H27" s="19" t="s">
         <v>31</v>
       </c>
@@ -4536,22 +4538,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
-    <col min="7" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" customWidth="1"/>
+    <col min="7" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="28" customFormat="1" ht="18">
+    <row r="1" spans="1:1024" s="28" customFormat="1" ht="17.399999999999999">
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
@@ -4982,7 +4984,9 @@
       <c r="D27" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="E27" s="37"/>
+      <c r="E27" s="37" t="s">
+        <v>87</v>
+      </c>
       <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6">
@@ -5791,18 +5795,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
-    <col min="7" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" customWidth="1"/>
+    <col min="7" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="28" customFormat="1" ht="18">
+    <row r="1" spans="1:1024" s="28" customFormat="1" ht="17.399999999999999">
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
@@ -6958,18 +6962,18 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
-    <col min="7" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" customWidth="1"/>
+    <col min="7" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="28" customFormat="1" ht="18">
+    <row r="1" spans="1:1024" s="28" customFormat="1" ht="17.399999999999999">
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
@@ -8125,18 +8129,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
-    <col min="7" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" customWidth="1"/>
+    <col min="7" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="28" customFormat="1" ht="18">
+    <row r="1" spans="1:1024" s="28" customFormat="1" ht="17.399999999999999">
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>
@@ -9292,18 +9296,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
-    <col min="7" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="51.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="6" max="6" width="51.88671875" customWidth="1"/>
+    <col min="7" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="28" customFormat="1" ht="18">
+    <row r="1" spans="1:1024" s="28" customFormat="1" ht="17.399999999999999">
       <c r="A1" s="26" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
elsa s01 final class written but not tested.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA.xlsx
+++ b/elsa/doc/Scrum_ELSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E6E301-9A45-4E79-A205-1CF5E37E6CA8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76CD0EF-7754-411F-B698-93AE03156B5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3048" yWindow="3048" windowWidth="17280" windowHeight="9108" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3048" yWindow="3048" windowWidth="17280" windowHeight="9108" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="89">
   <si>
     <t>Product Name:</t>
   </si>
@@ -299,7 +299,10 @@
     <t>Completed Day 3</t>
   </si>
   <si>
-    <t>In Work</t>
+    <t>In Test</t>
+  </si>
+  <si>
+    <t>Completed Day 4</t>
   </si>
 </sst>
 </file>
@@ -1075,16 +1078,16 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3028,7 +3031,7 @@
   </sheetPr>
   <dimension ref="A1:AMK96"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -4538,8 +4541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -4713,11 +4716,11 @@
       </c>
       <c r="B11" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C11" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -4731,7 +4734,7 @@
       </c>
       <c r="B12" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C12" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -4749,7 +4752,7 @@
       </c>
       <c r="B13" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C13" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -4767,7 +4770,7 @@
       </c>
       <c r="B14" s="33">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C14" s="26">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -4985,7 +4988,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F27" s="38"/>
     </row>
@@ -5000,7 +5003,9 @@
       <c r="D28" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="E28" s="37"/>
+      <c r="E28" s="37" t="s">
+        <v>88</v>
+      </c>
       <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6">
@@ -5014,7 +5019,9 @@
       <c r="D29" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="37"/>
+      <c r="E29" s="37" t="s">
+        <v>88</v>
+      </c>
       <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:6">
@@ -5028,7 +5035,9 @@
       <c r="D30" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="37"/>
+      <c r="E30" s="37" t="s">
+        <v>88</v>
+      </c>
       <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6">
@@ -5042,7 +5051,9 @@
       <c r="D31" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="E31" s="37"/>
+      <c r="E31" s="37" t="s">
+        <v>88</v>
+      </c>
       <c r="F31" s="38"/>
     </row>
     <row r="32" spans="1:6">
@@ -5056,7 +5067,9 @@
       <c r="D32" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="E32" s="37"/>
+      <c r="E32" s="37" t="s">
+        <v>88</v>
+      </c>
       <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:6">

</xml_diff>

<commit_message>
elsa s01 final completed.
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA.xlsx
+++ b/elsa/doc/Scrum_ELSA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gupta\Dropbox\CLASS UTA\Spring 2020\CSE 1325\VMShared\cse1325\elsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76CD0EF-7754-411F-B698-93AE03156B5B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB03F485-38E9-4343-8C80-D85C59282841}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3048" yWindow="3048" windowWidth="17280" windowHeight="9108" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="88">
   <si>
     <t>Product Name:</t>
   </si>
@@ -297,9 +297,6 @@
   </si>
   <si>
     <t>Completed Day 3</t>
-  </si>
-  <si>
-    <t>In Test</t>
   </si>
   <si>
     <t>Completed Day 4</t>
@@ -783,19 +780,19 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3031,8 +3028,8 @@
   </sheetPr>
   <dimension ref="A1:AMK96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3242,11 +3239,11 @@
       </c>
       <c r="B13" s="2">
         <f>B12-C13</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 1")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
@@ -3266,7 +3263,7 @@
       </c>
       <c r="B14" s="2">
         <f>B13-C14</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 2")</f>
@@ -3290,7 +3287,7 @@
       </c>
       <c r="B15" s="2">
         <f>B14-C15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 3")</f>
@@ -3314,7 +3311,7 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 4")</f>
@@ -3334,7 +3331,7 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="8">
         <f>COUNTIF(G$24:G$102,"Finished in Sprint 4")</f>
@@ -3525,7 +3522,9 @@
       <c r="E26" s="17">
         <v>8</v>
       </c>
-      <c r="F26" s="18"/>
+      <c r="F26" s="18">
+        <v>3</v>
+      </c>
       <c r="G26" s="18" t="s">
         <v>80</v>
       </c>
@@ -3554,9 +3553,11 @@
       <c r="E27" s="17">
         <v>13</v>
       </c>
-      <c r="F27" s="18"/>
+      <c r="F27" s="18">
+        <v>4</v>
+      </c>
       <c r="G27" s="18" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H27" s="19" t="s">
         <v>31</v>
@@ -4541,8 +4542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -4988,7 +4989,7 @@
         <v>73</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="38"/>
     </row>
@@ -5004,7 +5005,7 @@
         <v>74</v>
       </c>
       <c r="E28" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F28" s="38"/>
     </row>
@@ -5020,7 +5021,7 @@
         <v>75</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F29" s="38"/>
     </row>
@@ -5036,7 +5037,7 @@
         <v>76</v>
       </c>
       <c r="E30" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F30" s="38"/>
     </row>
@@ -5052,7 +5053,7 @@
         <v>77</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31" s="38"/>
     </row>
@@ -5068,7 +5069,7 @@
         <v>78</v>
       </c>
       <c r="E32" s="37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F32" s="38"/>
     </row>

</xml_diff>